<commit_message>
LessonCalendar state management is done. LessonModal readOnly mode in progress.
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Event Service Release.xlsx
+++ b/turbolessons-frontend/spec/Event Service Release.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FBF60-E555-3841-9205-95E8B00730B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B97B388-AAA1-454D-B20B-CBB1976386B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5520" yWindow="-28300" windowWidth="32820" windowHeight="27140" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -308,13 +308,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA8D3D-7358-DF48-915D-83CCC0E0788A}">
   <dimension ref="A2:A87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:A80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,7 +904,7 @@
       <c r="A72" s="1"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="5"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>

</xml_diff>

<commit_message>
edit/submit buttons in ui for LessonModal
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Event Service Release.xlsx
+++ b/turbolessons-frontend/spec/Event Service Release.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B97B388-AAA1-454D-B20B-CBB1976386B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C31448F-9748-4343-BC00-1E4CC7C92321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5520" yWindow="-28300" windowWidth="32820" windowHeight="27140" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Objective 2.1: Integrate Calendar View and Modal</t>
   </si>
@@ -243,6 +243,24 @@
   </si>
   <si>
     <t>form has appropriate buttons to edit or delete the lesson</t>
+  </si>
+  <si>
+    <t>User Changes duration option:</t>
+  </si>
+  <si>
+    <t>start time and end time are adjusted accordingly</t>
+  </si>
+  <si>
+    <t>User Changes Start Time</t>
+  </si>
+  <si>
+    <t>User changes end time:</t>
+  </si>
+  <si>
+    <t>start time is adjusted to appropriate value based on duration option</t>
+  </si>
+  <si>
+    <t>end time is adjusted to appropriate value based on duration option</t>
   </si>
 </sst>
 </file>
@@ -652,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA8D3D-7358-DF48-915D-83CCC0E0788A}">
-  <dimension ref="A2:A87"/>
+  <dimension ref="A2:A103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -937,6 +955,66 @@
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
     </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
handleDelete lesson is done
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Event Service Release.xlsx
+++ b/turbolessons-frontend/spec/Event Service Release.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C31448F-9748-4343-BC00-1E4CC7C92321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC764EF-5845-BE4B-A298-ACAE6309EF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5520" yWindow="-28300" windowWidth="32820" windowHeight="27140" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -670,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA8D3D-7358-DF48-915D-83CCC0E0788A}">
-  <dimension ref="A2:A103"/>
+  <dimension ref="A2:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -952,66 +952,63 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="5"/>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>44</v>
+      <c r="A93" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>48</v>
+      <c r="A98" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
passing isDateClick prop to LessonForm component
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Event Service Release.xlsx
+++ b/turbolessons-frontend/spec/Event Service Release.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC764EF-5845-BE4B-A298-ACAE6309EF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567C9A63-C964-FB41-A9DF-B87F1C999E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
+    <workbookView xWindow="-2180" yWindow="-28200" windowWidth="28340" windowHeight="20000" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Objective 2.1: Integrate Calendar View and Modal</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>end time is adjusted to appropriate value based on duration option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Case: </t>
+  </si>
+  <si>
+    <t>user performs write operations on a lesson (Edit/Delete) in LessonModal component</t>
+  </si>
+  <si>
+    <t>LessonCalendar Element updates when LessonModal Closes</t>
   </si>
 </sst>
 </file>
@@ -326,16 +335,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA8D3D-7358-DF48-915D-83CCC0E0788A}">
-  <dimension ref="A2:A101"/>
+  <dimension ref="A2:A106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -921,55 +927,70 @@
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
     </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="5"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+      <c r="A76" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
@@ -979,7 +1000,7 @@
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
@@ -989,7 +1010,7 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
@@ -999,7 +1020,7 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
@@ -1009,6 +1030,26 @@
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implement Fullcalendar API methods to handle LessonCalendar state changes, in progress
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Event Service Release.xlsx
+++ b/turbolessons-frontend/spec/Event Service Release.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567C9A63-C964-FB41-A9DF-B87F1C999E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3492FF-489E-0A46-B056-A795D5B8028A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2180" yWindow="-28200" windowWidth="28340" windowHeight="20000" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
+    <workbookView xWindow="1360" yWindow="-27740" windowWidth="28340" windowHeight="20000" xr2:uid="{8B77DE43-0577-AE46-A987-0F5D1D420877}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Objective 2.1: Integrate Calendar View and Modal</t>
   </si>
@@ -271,24 +271,39 @@
   <si>
     <t>LessonCalendar Element updates when LessonModal Closes</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ISSUE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> return states back to original when closing modals, etc.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF919288"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -335,13 +350,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,380 +690,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA8D3D-7358-DF48-915D-83CCC0E0788A}">
-  <dimension ref="A2:A106"/>
+  <dimension ref="A2:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
+      <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
+      <c r="A52" s="2"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
+      <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
+      <c r="A58" s="2"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
+      <c r="A62" s="2"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
+      <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+    <row r="80" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="5" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>